<commit_message>
Revised Rule Engine logic
</commit_message>
<xml_diff>
--- a/src/main/resources/persona.xlsx
+++ b/src/main/resources/persona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SnapFinance\git\neurosnap\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7676134E-6727-4647-91AD-224A4A4AA427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098D2888-07CB-4F0A-9D7E-7F42F8633237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F29E85F5-3592-4F04-9224-EEEC406E1D2D}"/>
   </bookViews>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF328F0-BCD4-411F-BE5A-9DED2A33F430}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +783,7 @@
         <v>5000</v>
       </c>
       <c r="H2" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I2" s="4">
         <v>3000</v>
@@ -842,7 +842,7 @@
         <v>3500</v>
       </c>
       <c r="H3" s="4">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I3" s="4">
         <v>2800</v>
@@ -901,7 +901,7 @@
         <v>1500</v>
       </c>
       <c r="H4" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="I4" s="4">
         <v>1200</v>
@@ -960,7 +960,7 @@
         <v>1000</v>
       </c>
       <c r="H5" s="4">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I5" s="4">
         <v>700</v>

</xml_diff>

<commit_message>
updating ssn in persona
</commit_message>
<xml_diff>
--- a/src/main/resources/persona.xlsx
+++ b/src/main/resources/persona.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SnapFinance\git\neurosnap\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D17215-535C-4A0B-B90B-EC572BA1841D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54952729-782E-4C5D-959E-1ECDAD8F1EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{F29E85F5-3592-4F04-9224-EEEC406E1D2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F29E85F5-3592-4F04-9224-EEEC406E1D2D}"/>
   </bookViews>
   <sheets>
     <sheet name="personas" sheetId="1" r:id="rId1"/>
@@ -328,13 +328,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -678,7 +678,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
         <v>29221</v>
       </c>
       <c r="L2" s="10">
-        <v>111111111</v>
+        <v>238435798</v>
       </c>
       <c r="M2" s="8">
         <v>9707101060</v>
@@ -854,7 +854,7 @@
         <v>29619</v>
       </c>
       <c r="L3" s="10">
-        <v>222222222</v>
+        <v>238435799</v>
       </c>
       <c r="M3" s="8">
         <v>9707101061</v>
@@ -913,7 +913,7 @@
         <v>30013</v>
       </c>
       <c r="L4" s="10">
-        <v>333333333</v>
+        <v>238435800</v>
       </c>
       <c r="M4" s="8">
         <v>9707101062</v>
@@ -972,7 +972,7 @@
         <v>30410</v>
       </c>
       <c r="L5" s="10">
-        <v>444444444</v>
+        <v>238435801</v>
       </c>
       <c r="M5" s="8">
         <v>9707101063</v>
@@ -1031,7 +1031,7 @@
         <v>30807</v>
       </c>
       <c r="L6" s="10">
-        <v>555555555</v>
+        <v>238435802</v>
       </c>
       <c r="M6" s="8">
         <v>9707101064</v>
@@ -1090,7 +1090,7 @@
         <v>31204</v>
       </c>
       <c r="L7" s="10">
-        <v>666666666</v>
+        <v>238435803</v>
       </c>
       <c r="M7" s="8">
         <v>9707101065</v>

</xml_diff>

<commit_message>
Generate plans using AI
</commit_message>
<xml_diff>
--- a/src/main/resources/persona.xlsx
+++ b/src/main/resources/persona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SnapFinance\git\neurosnap\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54952729-782E-4C5D-959E-1ECDAD8F1EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2A0F8-703D-41A8-AF8F-803AECE04A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F29E85F5-3592-4F04-9224-EEEC406E1D2D}"/>
   </bookViews>
@@ -678,7 +678,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new AI Recommand logic + Timeout Fix
</commit_message>
<xml_diff>
--- a/src/main/resources/persona.xlsx
+++ b/src/main/resources/persona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SnapFinance\git\neurosnap\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2A0F8-703D-41A8-AF8F-803AECE04A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5AAE96-0BA0-4725-AC3C-52D9E6EAF424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F29E85F5-3592-4F04-9224-EEEC406E1D2D}"/>
   </bookViews>
@@ -198,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +217,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -309,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,6 +349,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF328F0-BCD4-411F-BE5A-9DED2A33F430}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +974,7 @@
         <v>21</v>
       </c>
       <c r="F5" s="4">
-        <v>580</v>
+        <v>450</v>
       </c>
       <c r="G5" s="4">
         <v>1000</v>
@@ -1113,6 +1133,153 @@
       <c r="S7" s="8">
         <v>1610</v>
       </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="14"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="14"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="14"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="14"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="14"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating persona and token size
</commit_message>
<xml_diff>
--- a/src/main/resources/persona.xlsx
+++ b/src/main/resources/persona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SnapFinance\git\neurosnap\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E834AD-7729-4A19-96F7-B70F8EBB7526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E4E541-FB36-4217-951B-23AE4CAF37FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F29E85F5-3592-4F04-9224-EEEC406E1D2D}"/>
   </bookViews>
@@ -283,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -334,12 +334,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -679,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF328F0-BCD4-411F-BE5A-9DED2A33F430}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +688,7 @@
     <col min="6" max="6" width="12.5703125" style="8" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="20" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" style="2" customWidth="1"/>
@@ -703,7 +697,7 @@
     <col min="15" max="16" width="9.140625" style="8"/>
     <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.5703125" style="8" customWidth="1"/>
-    <col min="19" max="19" width="13" style="22" customWidth="1"/>
+    <col min="19" max="19" width="13" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.25">
@@ -1118,6 +1112,14 @@
       <c r="S7" s="19">
         <v>1360</v>
       </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I8"/>
+      <c r="S8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I9"/>
+      <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1128,7 +1130,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="20"/>
+      <c r="I10"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1138,7 +1140,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="20"/>
+      <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -1149,7 +1151,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="21"/>
+      <c r="I11"/>
       <c r="J11" s="4"/>
       <c r="K11" s="6"/>
       <c r="L11" s="4"/>
@@ -1159,7 +1161,7 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="17"/>
-      <c r="S11" s="21"/>
+      <c r="S11" s="8"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
@@ -1170,7 +1172,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="21"/>
+      <c r="I12"/>
       <c r="J12" s="4"/>
       <c r="K12" s="6"/>
       <c r="L12" s="4"/>
@@ -1180,7 +1182,7 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="17"/>
-      <c r="S12" s="21"/>
+      <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
@@ -1191,7 +1193,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="21"/>
+      <c r="I13"/>
       <c r="J13" s="4"/>
       <c r="K13" s="6"/>
       <c r="L13" s="4"/>
@@ -1201,7 +1203,7 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="17"/>
-      <c r="S13" s="21"/>
+      <c r="S13" s="8"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
@@ -1212,7 +1214,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="21"/>
+      <c r="I14"/>
       <c r="J14" s="4"/>
       <c r="K14" s="6"/>
       <c r="L14" s="4"/>
@@ -1222,7 +1224,7 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="17"/>
-      <c r="S14" s="21"/>
+      <c r="S14" s="8"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
@@ -1233,7 +1235,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="21"/>
+      <c r="I15"/>
       <c r="J15" s="4"/>
       <c r="K15" s="6"/>
       <c r="L15" s="4"/>
@@ -1243,7 +1245,7 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="17"/>
-      <c r="S15" s="21"/>
+      <c r="S15" s="8"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -1254,7 +1256,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="21"/>
+      <c r="I16"/>
       <c r="J16" s="4"/>
       <c r="K16" s="6"/>
       <c r="L16" s="4"/>
@@ -1264,7 +1266,326 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="7"/>
-      <c r="S16" s="21"/>
+      <c r="S16" s="8"/>
+    </row>
+    <row r="17" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I17"/>
+      <c r="S17" s="8"/>
+    </row>
+    <row r="18" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I18"/>
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I19"/>
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I20"/>
+      <c r="S20" s="8"/>
+    </row>
+    <row r="21" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I21"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I22"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I23"/>
+      <c r="S23" s="8"/>
+    </row>
+    <row r="24" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I24"/>
+      <c r="S24" s="8"/>
+    </row>
+    <row r="25" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I25"/>
+      <c r="S25" s="8"/>
+    </row>
+    <row r="26" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I26"/>
+      <c r="S26" s="8"/>
+    </row>
+    <row r="27" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I27"/>
+      <c r="S27" s="8"/>
+    </row>
+    <row r="28" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I28"/>
+      <c r="S28" s="8"/>
+    </row>
+    <row r="29" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I29"/>
+      <c r="S29" s="8"/>
+    </row>
+    <row r="30" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I30"/>
+      <c r="S30" s="8"/>
+    </row>
+    <row r="31" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I31"/>
+      <c r="S31" s="8"/>
+    </row>
+    <row r="32" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I32"/>
+      <c r="S32" s="8"/>
+    </row>
+    <row r="33" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I33"/>
+      <c r="S33" s="8"/>
+    </row>
+    <row r="34" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I34"/>
+      <c r="S34" s="8"/>
+    </row>
+    <row r="35" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I35"/>
+      <c r="S35" s="8"/>
+    </row>
+    <row r="36" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I36"/>
+      <c r="S36" s="8"/>
+    </row>
+    <row r="37" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I37"/>
+      <c r="S37" s="8"/>
+    </row>
+    <row r="38" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I38"/>
+      <c r="S38" s="8"/>
+    </row>
+    <row r="39" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I39"/>
+      <c r="S39" s="8"/>
+    </row>
+    <row r="40" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I40"/>
+      <c r="S40" s="8"/>
+    </row>
+    <row r="41" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I41"/>
+      <c r="S41" s="8"/>
+    </row>
+    <row r="42" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I42"/>
+      <c r="S42" s="8"/>
+    </row>
+    <row r="43" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I43"/>
+      <c r="S43" s="8"/>
+    </row>
+    <row r="44" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I44"/>
+      <c r="S44" s="8"/>
+    </row>
+    <row r="45" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I45"/>
+      <c r="S45" s="8"/>
+    </row>
+    <row r="46" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I46"/>
+      <c r="S46" s="8"/>
+    </row>
+    <row r="47" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I47"/>
+      <c r="S47" s="8"/>
+    </row>
+    <row r="48" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I48"/>
+      <c r="S48" s="8"/>
+    </row>
+    <row r="49" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I49"/>
+      <c r="S49" s="8"/>
+    </row>
+    <row r="50" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I50"/>
+      <c r="S50" s="8"/>
+    </row>
+    <row r="51" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I51"/>
+      <c r="S51" s="8"/>
+    </row>
+    <row r="52" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I52"/>
+      <c r="S52" s="8"/>
+    </row>
+    <row r="53" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I53"/>
+      <c r="S53" s="8"/>
+    </row>
+    <row r="54" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I54"/>
+      <c r="S54" s="8"/>
+    </row>
+    <row r="55" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I55"/>
+      <c r="S55" s="8"/>
+    </row>
+    <row r="56" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I56"/>
+      <c r="S56" s="8"/>
+    </row>
+    <row r="57" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I57"/>
+      <c r="S57" s="8"/>
+    </row>
+    <row r="58" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I58"/>
+      <c r="S58" s="8"/>
+    </row>
+    <row r="59" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I59"/>
+      <c r="S59" s="8"/>
+    </row>
+    <row r="60" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I60"/>
+      <c r="S60" s="8"/>
+    </row>
+    <row r="61" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I61"/>
+      <c r="S61" s="8"/>
+    </row>
+    <row r="62" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I62"/>
+      <c r="S62" s="8"/>
+    </row>
+    <row r="63" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I63"/>
+      <c r="S63" s="8"/>
+    </row>
+    <row r="64" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I64"/>
+      <c r="S64" s="8"/>
+    </row>
+    <row r="65" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I65"/>
+      <c r="S65" s="8"/>
+    </row>
+    <row r="66" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I66"/>
+      <c r="S66" s="8"/>
+    </row>
+    <row r="67" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I67"/>
+      <c r="S67" s="8"/>
+    </row>
+    <row r="68" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I68"/>
+      <c r="S68" s="8"/>
+    </row>
+    <row r="69" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I69"/>
+      <c r="S69" s="8"/>
+    </row>
+    <row r="70" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I70"/>
+      <c r="S70" s="8"/>
+    </row>
+    <row r="71" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I71"/>
+      <c r="S71" s="8"/>
+    </row>
+    <row r="72" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I72"/>
+      <c r="S72" s="8"/>
+    </row>
+    <row r="73" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I73"/>
+      <c r="S73" s="8"/>
+    </row>
+    <row r="74" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I74"/>
+      <c r="S74" s="8"/>
+    </row>
+    <row r="75" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I75"/>
+      <c r="S75" s="8"/>
+    </row>
+    <row r="76" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I76"/>
+      <c r="S76" s="8"/>
+    </row>
+    <row r="77" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I77"/>
+      <c r="S77" s="8"/>
+    </row>
+    <row r="78" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I78"/>
+      <c r="S78" s="8"/>
+    </row>
+    <row r="79" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I79"/>
+      <c r="S79" s="8"/>
+    </row>
+    <row r="80" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I80"/>
+      <c r="S80" s="8"/>
+    </row>
+    <row r="81" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I81"/>
+      <c r="S81" s="8"/>
+    </row>
+    <row r="82" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I82"/>
+      <c r="S82" s="8"/>
+    </row>
+    <row r="83" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I83"/>
+      <c r="S83" s="8"/>
+    </row>
+    <row r="84" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I84"/>
+      <c r="S84" s="8"/>
+    </row>
+    <row r="85" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I85"/>
+      <c r="S85" s="8"/>
+    </row>
+    <row r="86" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I86"/>
+      <c r="S86" s="8"/>
+    </row>
+    <row r="87" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I87"/>
+      <c r="S87" s="8"/>
+    </row>
+    <row r="88" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I88"/>
+      <c r="S88" s="8"/>
+    </row>
+    <row r="89" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I89"/>
+      <c r="S89" s="8"/>
+    </row>
+    <row r="90" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I90"/>
+      <c r="S90" s="8"/>
+    </row>
+    <row r="91" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I91"/>
+      <c r="S91" s="8"/>
+    </row>
+    <row r="92" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I92"/>
+      <c r="S92" s="8"/>
+    </row>
+    <row r="93" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I93"/>
+      <c r="S93" s="8"/>
+    </row>
+    <row r="94" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I94"/>
+      <c r="S94" s="8"/>
+    </row>
+    <row r="95" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I95"/>
+      <c r="S95" s="8"/>
+    </row>
+    <row r="96" spans="9:19" x14ac:dyDescent="0.25">
+      <c r="I96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding check for min tenure and adding income column in persona
</commit_message>
<xml_diff>
--- a/src/main/resources/persona.xlsx
+++ b/src/main/resources/persona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\SnapFinance\git\neurosnap\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADCE0FA-1D8C-455A-AC59-9502D207CD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D78E15-DB1F-4E9D-A1DA-B63769204F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F29E85F5-3592-4F04-9224-EEEC406E1D2D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t xml:space="preserve">Persona ID </t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>MRE</t>
+  </si>
+  <si>
+    <t>Income Amount</t>
+  </si>
+  <si>
+    <t>P_H_IRREGULAR_44</t>
+  </si>
+  <si>
+    <t>Henry Shah</t>
   </si>
 </sst>
 </file>
@@ -283,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,14 +328,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -339,6 +343,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF328F0-BCD4-411F-BE5A-9DED2A33F430}">
-  <dimension ref="A1:S96"/>
+  <dimension ref="A1:T96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,19 +715,20 @@
     <col min="6" max="6" width="12.5703125" style="8" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="23" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="13" max="13" width="16" style="18" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" style="8" customWidth="1"/>
     <col min="15" max="16" width="9.140625" style="8"/>
     <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" style="8" customWidth="1"/>
-    <col min="19" max="19" width="13" style="20" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" style="8" customWidth="1"/>
+    <col min="19" max="19" width="13" style="17" customWidth="1"/>
+    <col min="20" max="20" width="21.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +753,7 @@
       <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="21" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -737,7 +765,7 @@
       <c r="L1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="24" t="s">
         <v>41</v>
       </c>
       <c r="N1" s="9" t="s">
@@ -755,11 +783,14 @@
       <c r="R1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -784,19 +815,19 @@
       <c r="H2" s="12">
         <v>12</v>
       </c>
-      <c r="I2" s="19">
+      <c r="I2" s="22">
         <v>2500</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="20">
         <v>29221</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="13">
         <v>238435798</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="25">
         <v>9707101060</v>
       </c>
       <c r="N2" s="12">
@@ -808,17 +839,20 @@
       <c r="P2" s="12">
         <v>437</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Q2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="16">
+      <c r="R2" s="19">
         <v>234565009001</v>
       </c>
-      <c r="S2" s="19">
+      <c r="S2" s="16">
         <v>2610</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="T2" s="16">
+        <v>85000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
@@ -843,19 +877,19 @@
       <c r="H3" s="12">
         <v>18</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="22">
         <v>1750</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="20">
         <v>29619</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="13">
         <v>238435799</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="25">
         <v>9707101061</v>
       </c>
       <c r="N3" s="12">
@@ -867,17 +901,20 @@
       <c r="P3" s="12">
         <v>314</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R3" s="19">
         <v>234565009002</v>
       </c>
-      <c r="S3" s="19">
+      <c r="S3" s="16">
         <v>1860</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="T3" s="16">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
@@ -902,19 +939,19 @@
       <c r="H4" s="12">
         <v>12</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="22">
         <v>750</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="20">
         <v>30013</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="13">
         <v>238435800</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="25">
         <v>9707101062</v>
       </c>
       <c r="N4" s="12">
@@ -926,17 +963,20 @@
       <c r="P4" s="12">
         <v>267</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="16">
+      <c r="R4" s="19">
         <v>234565009003</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="16">
         <v>860</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="T4" s="16">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>19</v>
       </c>
@@ -961,19 +1001,19 @@
       <c r="H5" s="12">
         <v>30</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="22">
         <v>500</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="20">
         <v>30410</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <v>238435801</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="25">
         <v>9707101063</v>
       </c>
       <c r="N5" s="12">
@@ -985,17 +1025,20 @@
       <c r="P5" s="12">
         <v>192</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="R5" s="16">
+      <c r="R5" s="19">
         <v>234565009004</v>
       </c>
-      <c r="S5" s="19">
+      <c r="S5" s="16">
         <v>610</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="T5" s="16">
+        <v>29000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
@@ -1020,19 +1063,19 @@
       <c r="H6" s="12">
         <v>12</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="22">
         <v>2000</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="20">
         <v>30807</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <v>238435802</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="25">
         <v>9707101064</v>
       </c>
       <c r="N6" s="12">
@@ -1044,17 +1087,20 @@
       <c r="P6" s="12">
         <v>355</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="16">
+      <c r="R6" s="19">
         <v>234565009005</v>
       </c>
-      <c r="S6" s="19">
+      <c r="S6" s="16">
         <v>2110</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="T6" s="16">
+        <v>87000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>25</v>
       </c>
@@ -1079,19 +1125,19 @@
       <c r="H7" s="12">
         <v>16</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="22">
         <v>1250</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="20">
         <v>31204</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="13">
         <v>238435803</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="25">
         <v>9707101065</v>
       </c>
       <c r="N7" s="12">
@@ -1103,25 +1149,86 @@
       <c r="P7" s="12">
         <v>223</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="Q7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="19">
         <v>234565009006</v>
       </c>
-      <c r="S7" s="19">
+      <c r="S7" s="16">
         <v>1360</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I8"/>
-      <c r="S8" s="8"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I9"/>
+      <c r="T7" s="16">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="12">
+        <v>600</v>
+      </c>
+      <c r="G8" s="12">
+        <v>3000</v>
+      </c>
+      <c r="H8" s="12">
+        <v>19</v>
+      </c>
+      <c r="I8" s="22">
+        <v>2000</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="20">
+        <v>31569</v>
+      </c>
+      <c r="L8" s="13">
+        <v>238435804</v>
+      </c>
+      <c r="M8" s="25">
+        <v>9707101066</v>
+      </c>
+      <c r="N8" s="12">
+        <v>7777</v>
+      </c>
+      <c r="O8" s="12">
+        <v>12</v>
+      </c>
+      <c r="P8" s="12">
+        <v>267</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="R8" s="19">
+        <v>234565009006</v>
+      </c>
+      <c r="S8" s="16">
+        <v>2160</v>
+      </c>
+      <c r="T8" s="16">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I9" s="2"/>
       <c r="S9" s="8"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1130,11 +1237,11 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="M10" s="5"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
@@ -1142,7 +1249,7 @@
       <c r="R10" s="3"/>
       <c r="S10" s="8"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
@@ -1151,7 +1258,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="4"/>
       <c r="K11" s="6"/>
       <c r="L11" s="4"/>
@@ -1160,10 +1267,10 @@
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="17"/>
+      <c r="R11" s="14"/>
       <c r="S11" s="8"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
@@ -1172,7 +1279,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12"/>
+      <c r="I12" s="2"/>
       <c r="J12" s="4"/>
       <c r="K12" s="6"/>
       <c r="L12" s="4"/>
@@ -1181,10 +1288,10 @@
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="17"/>
+      <c r="R12" s="14"/>
       <c r="S12" s="8"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4"/>
@@ -1193,7 +1300,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="4"/>
       <c r="K13" s="6"/>
       <c r="L13" s="4"/>
@@ -1202,10 +1309,10 @@
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="17"/>
+      <c r="R13" s="14"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="4"/>
@@ -1214,7 +1321,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="4"/>
       <c r="K14" s="6"/>
       <c r="L14" s="4"/>
@@ -1223,10 +1330,10 @@
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="17"/>
+      <c r="R14" s="14"/>
       <c r="S14" s="8"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="4"/>
@@ -1235,7 +1342,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="4"/>
       <c r="K15" s="6"/>
       <c r="L15" s="4"/>
@@ -1244,10 +1351,10 @@
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="4"/>
-      <c r="R15" s="17"/>
+      <c r="R15" s="14"/>
       <c r="S15" s="8"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="4"/>
@@ -1256,7 +1363,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16"/>
+      <c r="I16" s="2"/>
       <c r="J16" s="4"/>
       <c r="K16" s="6"/>
       <c r="L16" s="4"/>
@@ -1269,323 +1376,323 @@
       <c r="S16" s="8"/>
     </row>
     <row r="17" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I17"/>
+      <c r="I17" s="2"/>
       <c r="S17" s="8"/>
     </row>
     <row r="18" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I18"/>
+      <c r="I18" s="2"/>
       <c r="S18" s="8"/>
     </row>
     <row r="19" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I19"/>
+      <c r="I19" s="2"/>
       <c r="S19" s="8"/>
     </row>
     <row r="20" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I20"/>
+      <c r="I20" s="2"/>
       <c r="S20" s="8"/>
     </row>
     <row r="21" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I21"/>
+      <c r="I21" s="2"/>
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I22"/>
+      <c r="I22" s="2"/>
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I23"/>
+      <c r="I23" s="2"/>
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I24"/>
+      <c r="I24" s="2"/>
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I25"/>
+      <c r="I25" s="2"/>
       <c r="S25" s="8"/>
     </row>
     <row r="26" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I26"/>
+      <c r="I26" s="2"/>
       <c r="S26" s="8"/>
     </row>
     <row r="27" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I27"/>
+      <c r="I27" s="2"/>
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I28"/>
+      <c r="I28" s="2"/>
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I29"/>
+      <c r="I29" s="2"/>
       <c r="S29" s="8"/>
     </row>
     <row r="30" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I30"/>
+      <c r="I30" s="2"/>
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I31"/>
+      <c r="I31" s="2"/>
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I32"/>
+      <c r="I32" s="2"/>
       <c r="S32" s="8"/>
     </row>
     <row r="33" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I33"/>
+      <c r="I33" s="2"/>
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I34"/>
+      <c r="I34" s="2"/>
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I35"/>
+      <c r="I35" s="2"/>
       <c r="S35" s="8"/>
     </row>
     <row r="36" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I36"/>
+      <c r="I36" s="2"/>
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I37"/>
+      <c r="I37" s="2"/>
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I38"/>
+      <c r="I38" s="2"/>
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I39"/>
+      <c r="I39" s="2"/>
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I40"/>
+      <c r="I40" s="2"/>
       <c r="S40" s="8"/>
     </row>
     <row r="41" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I41"/>
+      <c r="I41" s="2"/>
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I42"/>
+      <c r="I42" s="2"/>
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I43"/>
+      <c r="I43" s="2"/>
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I44"/>
+      <c r="I44" s="2"/>
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I45"/>
+      <c r="I45" s="2"/>
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I46"/>
+      <c r="I46" s="2"/>
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I47"/>
+      <c r="I47" s="2"/>
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I48"/>
+      <c r="I48" s="2"/>
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I49"/>
+      <c r="I49" s="2"/>
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I50"/>
+      <c r="I50" s="2"/>
       <c r="S50" s="8"/>
     </row>
     <row r="51" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I51"/>
+      <c r="I51" s="2"/>
       <c r="S51" s="8"/>
     </row>
     <row r="52" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I52"/>
+      <c r="I52" s="2"/>
       <c r="S52" s="8"/>
     </row>
     <row r="53" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I53"/>
+      <c r="I53" s="2"/>
       <c r="S53" s="8"/>
     </row>
     <row r="54" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I54"/>
+      <c r="I54" s="2"/>
       <c r="S54" s="8"/>
     </row>
     <row r="55" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I55"/>
+      <c r="I55" s="2"/>
       <c r="S55" s="8"/>
     </row>
     <row r="56" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I56"/>
+      <c r="I56" s="2"/>
       <c r="S56" s="8"/>
     </row>
     <row r="57" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I57"/>
+      <c r="I57" s="2"/>
       <c r="S57" s="8"/>
     </row>
     <row r="58" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I58"/>
+      <c r="I58" s="2"/>
       <c r="S58" s="8"/>
     </row>
     <row r="59" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I59"/>
+      <c r="I59" s="2"/>
       <c r="S59" s="8"/>
     </row>
     <row r="60" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I60"/>
+      <c r="I60" s="2"/>
       <c r="S60" s="8"/>
     </row>
     <row r="61" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I61"/>
+      <c r="I61" s="2"/>
       <c r="S61" s="8"/>
     </row>
     <row r="62" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I62"/>
+      <c r="I62" s="2"/>
       <c r="S62" s="8"/>
     </row>
     <row r="63" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I63"/>
+      <c r="I63" s="2"/>
       <c r="S63" s="8"/>
     </row>
     <row r="64" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I64"/>
+      <c r="I64" s="2"/>
       <c r="S64" s="8"/>
     </row>
     <row r="65" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I65"/>
+      <c r="I65" s="2"/>
       <c r="S65" s="8"/>
     </row>
     <row r="66" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I66"/>
+      <c r="I66" s="2"/>
       <c r="S66" s="8"/>
     </row>
     <row r="67" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I67"/>
+      <c r="I67" s="2"/>
       <c r="S67" s="8"/>
     </row>
     <row r="68" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I68"/>
+      <c r="I68" s="2"/>
       <c r="S68" s="8"/>
     </row>
     <row r="69" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I69"/>
+      <c r="I69" s="2"/>
       <c r="S69" s="8"/>
     </row>
     <row r="70" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I70"/>
+      <c r="I70" s="2"/>
       <c r="S70" s="8"/>
     </row>
     <row r="71" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I71"/>
+      <c r="I71" s="2"/>
       <c r="S71" s="8"/>
     </row>
     <row r="72" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I72"/>
+      <c r="I72" s="2"/>
       <c r="S72" s="8"/>
     </row>
     <row r="73" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I73"/>
+      <c r="I73" s="2"/>
       <c r="S73" s="8"/>
     </row>
     <row r="74" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I74"/>
+      <c r="I74" s="2"/>
       <c r="S74" s="8"/>
     </row>
     <row r="75" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I75"/>
+      <c r="I75" s="2"/>
       <c r="S75" s="8"/>
     </row>
     <row r="76" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I76"/>
+      <c r="I76" s="2"/>
       <c r="S76" s="8"/>
     </row>
     <row r="77" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I77"/>
+      <c r="I77" s="2"/>
       <c r="S77" s="8"/>
     </row>
     <row r="78" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I78"/>
+      <c r="I78" s="2"/>
       <c r="S78" s="8"/>
     </row>
     <row r="79" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I79"/>
+      <c r="I79" s="2"/>
       <c r="S79" s="8"/>
     </row>
     <row r="80" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I80"/>
+      <c r="I80" s="2"/>
       <c r="S80" s="8"/>
     </row>
     <row r="81" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I81"/>
+      <c r="I81" s="2"/>
       <c r="S81" s="8"/>
     </row>
     <row r="82" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I82"/>
+      <c r="I82" s="2"/>
       <c r="S82" s="8"/>
     </row>
     <row r="83" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I83"/>
+      <c r="I83" s="2"/>
       <c r="S83" s="8"/>
     </row>
     <row r="84" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I84"/>
+      <c r="I84" s="2"/>
       <c r="S84" s="8"/>
     </row>
     <row r="85" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I85"/>
+      <c r="I85" s="2"/>
       <c r="S85" s="8"/>
     </row>
     <row r="86" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I86"/>
+      <c r="I86" s="2"/>
       <c r="S86" s="8"/>
     </row>
     <row r="87" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I87"/>
+      <c r="I87" s="2"/>
       <c r="S87" s="8"/>
     </row>
     <row r="88" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I88"/>
+      <c r="I88" s="2"/>
       <c r="S88" s="8"/>
     </row>
     <row r="89" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I89"/>
+      <c r="I89" s="2"/>
       <c r="S89" s="8"/>
     </row>
     <row r="90" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I90"/>
+      <c r="I90" s="2"/>
       <c r="S90" s="8"/>
     </row>
     <row r="91" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I91"/>
+      <c r="I91" s="2"/>
       <c r="S91" s="8"/>
     </row>
     <row r="92" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I92"/>
+      <c r="I92" s="2"/>
       <c r="S92" s="8"/>
     </row>
     <row r="93" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I93"/>
+      <c r="I93" s="2"/>
       <c r="S93" s="8"/>
     </row>
     <row r="94" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I94"/>
+      <c r="I94" s="2"/>
       <c r="S94" s="8"/>
     </row>
     <row r="95" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I95"/>
+      <c r="I95" s="2"/>
       <c r="S95" s="8"/>
     </row>
     <row r="96" spans="9:19" x14ac:dyDescent="0.25">
-      <c r="I96"/>
+      <c r="I96" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>